<commit_message>
shifted forward mumbai dates
</commit_message>
<xml_diff>
--- a/dataset/19_ROIs.xlsx
+++ b/dataset/19_ROIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\TemporalGAN\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8CA5FA-A02D-482A-A7B3-AA73DFD429AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E22A2CD-4DED-49D1-A9E4-3DF2E146E033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -366,9 +366,6 @@
     <t>('2019-07-07','2019-08-07')</t>
   </si>
   <si>
-    <t>('2019-01-07','2019-02-07')</t>
-  </si>
-  <si>
     <t>train_test</t>
   </si>
   <si>
@@ -376,6 +373,9 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>('2019-03-07','2019-04-07')</t>
   </si>
 </sst>
 </file>
@@ -1071,7 +1071,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1125,7 +1125,7 @@
         <v>10</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>11</v>
@@ -1180,7 +1180,7 @@
         <v>16</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
@@ -1233,7 +1233,7 @@
         <v>19</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
@@ -1286,7 +1286,7 @@
         <v>22</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
@@ -1339,7 +1339,7 @@
         <v>16</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
@@ -1392,7 +1392,7 @@
         <v>19</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
@@ -1445,7 +1445,7 @@
         <v>22</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
@@ -1498,7 +1498,7 @@
         <v>16</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
@@ -1551,7 +1551,7 @@
         <v>22</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
@@ -1604,7 +1604,7 @@
         <v>16</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>36</v>
@@ -1659,7 +1659,7 @@
         <v>19</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M11" s="4" t="s">
         <v>36</v>
@@ -1714,7 +1714,7 @@
         <v>16</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>41</v>
@@ -1769,7 +1769,7 @@
         <v>19</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>41</v>
@@ -1824,7 +1824,7 @@
         <v>16</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
@@ -1877,7 +1877,7 @@
         <v>19</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
@@ -1930,7 +1930,7 @@
         <v>16</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
@@ -1983,7 +1983,7 @@
         <v>22</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
@@ -2036,7 +2036,7 @@
         <v>16</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
@@ -2089,7 +2089,7 @@
         <v>19</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
@@ -2142,7 +2142,7 @@
         <v>22</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
@@ -2195,7 +2195,7 @@
         <v>16</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
@@ -2248,7 +2248,7 @@
         <v>19</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
@@ -2301,7 +2301,7 @@
         <v>22</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
@@ -2354,7 +2354,7 @@
         <v>16</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M24" s="4" t="s">
         <v>65</v>
@@ -2409,7 +2409,7 @@
         <v>22</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
@@ -2462,7 +2462,7 @@
         <v>16</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
@@ -2515,7 +2515,7 @@
         <v>19</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M27" s="4" t="s">
         <v>72</v>
@@ -2570,7 +2570,7 @@
         <v>16</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
@@ -2623,7 +2623,7 @@
         <v>19</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
@@ -2676,7 +2676,7 @@
         <v>16</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
@@ -2729,7 +2729,7 @@
         <v>19</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
@@ -2758,7 +2758,7 @@
         <v>82</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>14</v>
@@ -2782,7 +2782,7 @@
         <v>16</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
@@ -2811,7 +2811,7 @@
         <v>84</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>14</v>
@@ -2835,7 +2835,7 @@
         <v>19</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
@@ -2888,7 +2888,7 @@
         <v>16</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
@@ -2941,7 +2941,7 @@
         <v>19</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
@@ -2994,7 +2994,7 @@
         <v>16</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
@@ -3047,7 +3047,7 @@
         <v>16</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
@@ -3100,7 +3100,7 @@
         <v>19</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
@@ -3153,7 +3153,7 @@
         <v>16</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
@@ -3206,7 +3206,7 @@
         <v>16</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
@@ -3259,7 +3259,7 @@
         <v>16</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M41" s="4" t="s">
         <v>101</v>
@@ -3314,7 +3314,7 @@
         <v>16</v>
       </c>
       <c r="L42" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
@@ -3367,7 +3367,7 @@
         <v>16</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M43" s="4"/>
       <c r="N43" s="4"/>
@@ -3420,7 +3420,7 @@
         <v>16</v>
       </c>
       <c r="L44" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
@@ -3473,7 +3473,7 @@
         <v>19</v>
       </c>
       <c r="L45" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M45" s="4"/>
       <c r="N45" s="4"/>

</xml_diff>